<commit_message>
Agregada función de dias para fecha límite
</commit_message>
<xml_diff>
--- a/avances_de_proyecto/avance2/Diccionario de datos.xlsx
+++ b/avances_de_proyecto/avance2/Diccionario de datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiri\Documents\Tec\4\Construcción de Software y Toma de Desiciones\CADCE\avances_de_proyecto\avance2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4204AD5-2D36-4E53-9DDC-59F0E7F16C49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A225E0-6DC5-4792-8621-595398D924EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FD2593C4-7468-428B-B6D4-5A6EDBFFA527}"/>
+    <workbookView xWindow="9540" yWindow="468" windowWidth="12516" windowHeight="8964" xr2:uid="{FD2593C4-7468-428B-B6D4-5A6EDBFFA527}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
   <si>
     <t>Nombre del Atributo</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Caracteres(50)</t>
   </si>
   <si>
-    <t>Descripción de la función</t>
-  </si>
-  <si>
     <t>Caracteres(100)</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>Implementación del archivo XXXX</t>
   </si>
   <si>
-    <t>Terminar el archivo XXXX que permitirá el inicio de sesión en conjunto a YYYY</t>
-  </si>
-  <si>
     <t>Entidad Empleado</t>
   </si>
   <si>
@@ -277,6 +271,15 @@
   </si>
   <si>
     <t>Número de versión del caso de uso</t>
+  </si>
+  <si>
+    <t>Fase</t>
+  </si>
+  <si>
+    <t>Fase en la que se ecuentra la tarea</t>
+  </si>
+  <si>
+    <t>El archivo XXXX se encuentra en Fase YYYY</t>
   </si>
 </sst>
 </file>
@@ -519,9 +522,7 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
+        <right/>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -554,7 +555,9 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -598,6 +601,56 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -633,56 +686,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -1711,14 +1714,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5D9E9C8C-803B-49BF-9DE0-78C46E7376AE}" name="Tabla6" displayName="Tabla6" ref="A12:E19" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5D9E9C8C-803B-49BF-9DE0-78C46E7376AE}" name="Tabla6" displayName="Tabla6" ref="A12:E19" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A12:E19" xr:uid="{A8A03E47-B44C-4F9D-BC3C-515170B3A5A6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{56C6DA02-6BB2-477B-916B-3CF19CAE516D}" name="Nombre del Atributo" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{56C6DA02-6BB2-477B-916B-3CF19CAE516D}" name="Nombre del Atributo" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{62B2E32A-C44B-4D3A-B3D3-247564FD43F9}" name="Descripción"/>
-    <tableColumn id="3" xr3:uid="{7AE8BFB6-1F41-45A7-8083-588783167076}" name="Tipo de dato" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{E87C90F1-9873-468E-B59F-4C75AB3634DE}" name="Null or Not Null" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1D3597C8-FDAE-46A1-87BF-665AC8409B72}" name="Ejemplo" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7AE8BFB6-1F41-45A7-8083-588783167076}" name="Tipo de dato" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{E87C90F1-9873-468E-B59F-4C75AB3634DE}" name="Null or Not Null" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1D3597C8-FDAE-46A1-87BF-665AC8409B72}" name="Ejemplo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2023,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD8A156-4755-45B5-93CA-17EB58A7C866}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2042,7 +2045,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2183,7 +2186,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2205,10 +2208,10 @@
     </row>
     <row r="13" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>30</v>
@@ -2217,7 +2220,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -2225,7 +2228,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>11</v>
@@ -2234,7 +2237,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
@@ -2251,12 +2254,12 @@
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>43</v>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>47</v>
@@ -2290,13 +2293,13 @@
     </row>
     <row r="18" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>8</v>
@@ -2307,13 +2310,13 @@
     </row>
     <row r="19" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
@@ -2324,7 +2327,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2346,10 +2349,10 @@
     </row>
     <row r="23" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>7</v>
@@ -2358,15 +2361,15 @@
         <v>8</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>7</v>
@@ -2375,7 +2378,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -2392,24 +2395,24 @@
         <v>8</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -2448,7 +2451,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2504,7 +2507,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>20</v>
@@ -2521,7 +2524,7 @@
     </row>
     <row r="35" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>10</v>
@@ -2533,7 +2536,7 @@
         <v>8</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -2555,7 +2558,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>